<commit_message>
Atualização do backlog semanal
</commit_message>
<xml_diff>
--- a/Documentação/backLogs e Planos de ação/planoDeAção BackLog PlanilhaDeRiscos.xlsx
+++ b/Documentação/backLogs e Planos de ação/planoDeAção BackLog PlanilhaDeRiscos.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27016"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pehso\Downloads\git clone(2)\MushRoomCompany\Documentação\backLogs e Planos de ação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Desktop\Material Sptech\Projetos\MushRoomCompany\Documentação\backLogs e Planos de ação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BE6C2BB-149A-4F62-B9D0-3121BDBA4FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BackLogs" sheetId="4" r:id="rId1"/>
     <sheet name="Planilha de Riscos" sheetId="2" r:id="rId2"/>
     <sheet name="Plano de Ação" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,14 +37,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="235">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -721,9 +720,6 @@
     <t>Daniel</t>
   </si>
   <si>
-    <t>“Projeto do site”</t>
-  </si>
-  <si>
     <t>Pedro</t>
   </si>
   <si>
@@ -731,16 +727,55 @@
   </si>
   <si>
     <t>Leonardo</t>
+  </si>
+  <si>
+    <t>Criar o CSS e o HTML do Detalhes do projeto</t>
+  </si>
+  <si>
+    <t>Criar o css e html do footer e implementar no site</t>
+  </si>
+  <si>
+    <t>Fazer o CSS e o HTML da Dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar o Script de validação das inputs e e mensagem de erro </t>
+  </si>
+  <si>
+    <t>Tela Sobre nós</t>
+  </si>
+  <si>
+    <t>Fazer o CSS e o HTML da sobre nós</t>
+  </si>
+  <si>
+    <t>Modificar o codigo da API para que ele interaja com o banco de dados</t>
+  </si>
+  <si>
+    <t>Scrum Master SP2D: Matteus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definir os graficos </t>
+  </si>
+  <si>
+    <t>Diagrama de solução</t>
+  </si>
+  <si>
+    <t>Escrever legenda no Diagrama de solução</t>
+  </si>
+  <si>
+    <t>Arrumar logica da calculadora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modulo analytics </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -869,12 +904,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Merriweather"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="40">
@@ -1113,7 +1142,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1349,11 +1378,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1595,6 +1639,30 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="32" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1664,26 +1732,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="31" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="32" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="31" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1691,25 +1756,12 @@
     <xf numFmtId="0" fontId="7" fillId="30" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1806,7 +1858,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1873,7 +1925,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -2030,7 +2082,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="819904352"/>
@@ -2099,7 +2151,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="814723552"/>
@@ -2143,7 +2195,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3048,7 +3100,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC1444C-8C51-4391-AC27-3F562DB04093}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X73"/>
   <sheetViews>
     <sheetView topLeftCell="B33" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
@@ -3084,31 +3136,31 @@
   <sheetData>
     <row r="1" spans="1:24" ht="53.25" customHeight="1">
       <c r="A1" s="8"/>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="88"/>
-      <c r="L1" s="81" t="s">
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="96"/>
+      <c r="L1" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="90"/>
+      <c r="S1" s="90"/>
+      <c r="T1" s="90"/>
+      <c r="U1" s="90"/>
+      <c r="V1" s="90"/>
+      <c r="W1" s="90"/>
+      <c r="X1" s="90"/>
     </row>
     <row r="2" spans="1:24" ht="27.95" customHeight="1">
       <c r="A2" s="3" t="s">
@@ -3289,57 +3341,57 @@
         <v>163</v>
       </c>
       <c r="N4" s="67" cm="1">
-        <f t="array" ref="N4">IF(SUM(N3)&gt;0,M4-N3,_xludf.n
+        <f t="array" ref="N4">IF(SUM(N3)&gt;0,M4-N3,n
 )</f>
         <v>147</v>
       </c>
       <c r="O4" s="67" cm="1">
-        <f t="array" ref="O4">IF(SUM(O3)&gt;0,N4-O3,_xludf.n
+        <f t="array" ref="O4">IF(SUM(O3)&gt;0,N4-O3,n
 )</f>
         <v>130</v>
       </c>
       <c r="P4" s="67" cm="1">
-        <f t="array" ref="P4">IF(SUM(P3)&gt;0,O4-P3,_xludf.n
+        <f t="array" ref="P4">IF(SUM(P3)&gt;0,O4-P3,n
 )</f>
         <v>112</v>
       </c>
       <c r="Q4" s="67" cm="1">
-        <f t="array" ref="Q4">IF(SUM(Q3)&gt;0,P4-Q3,_xludf.n
+        <f t="array" ref="Q4">IF(SUM(Q3)&gt;0,P4-Q3,n
 )</f>
         <v>95</v>
       </c>
       <c r="R4" s="67" cm="1">
-        <f t="array" ref="R4">IF(SUM(R3)&gt;0,Q4-R3,_xludf.n
+        <f t="array" ref="R4">IF(SUM(R3)&gt;0,Q4-R3,n
 )</f>
         <v>80</v>
       </c>
       <c r="S4" s="67" cm="1">
-        <f t="array" ref="S4">IF(SUM(S3)&gt;0,R4-S3,_xludf.n
+        <f t="array" ref="S4">IF(SUM(S3)&gt;0,R4-S3,n
 )</f>
         <v>64</v>
       </c>
       <c r="T4" s="67" cm="1">
-        <f t="array" ref="T4">IF(SUM(T3)&gt;0,S4-T3,_xludf.n
+        <f t="array" ref="T4">IF(SUM(T3)&gt;0,S4-T3,n
 )</f>
         <v>47</v>
       </c>
       <c r="U4" s="67" cm="1">
-        <f t="array" ref="U4">IF(SUM(U3)&gt;0,T4-U3,_xludf.n
+        <f t="array" ref="U4">IF(SUM(U3)&gt;0,T4-U3,n
 )</f>
         <v>31</v>
       </c>
       <c r="V4" s="67" cm="1">
-        <f t="array" ref="V4">IF(SUM(V3)&gt;0,U4-V3,_xludf.n
+        <f t="array" ref="V4">IF(SUM(V3)&gt;0,U4-V3,n
 )</f>
         <v>16</v>
       </c>
       <c r="W4" s="67" cm="1">
-        <f t="array" ref="W4">IF(SUM(W3)&gt;0,V4-W3,_xludf.n
+        <f t="array" ref="W4">IF(SUM(W3)&gt;0,V4-W3,n
 )</f>
         <v>0</v>
       </c>
       <c r="X4" s="67" t="e" cm="1">
-        <f t="array" ref="X4">IF(SUM(X3)&gt;0,W4-X3,_xludf.n
+        <f t="array" ref="X4">IF(SUM(X3)&gt;0,W4-X3,n
 )</f>
         <v>#NAME?</v>
       </c>
@@ -3416,44 +3468,44 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="27.95" customHeight="1">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="91" t="s">
+      <c r="C7" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="93" t="s">
+      <c r="E7" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="90" t="s">
+      <c r="F7" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="90">
+      <c r="G7" s="98">
         <v>8</v>
       </c>
-      <c r="H7" s="89">
+      <c r="H7" s="97">
         <v>4</v>
       </c>
-      <c r="I7" s="96" t="s">
+      <c r="I7" s="104" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="27.95" customHeight="1">
-      <c r="A8" s="95"/>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="97"/>
+      <c r="A8" s="103"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="105"/>
     </row>
     <row r="9" spans="1:24" ht="27.95" customHeight="1">
       <c r="A9" s="11" t="s">
@@ -4169,17 +4221,17 @@
     </row>
     <row r="34" spans="1:10" ht="30.75" customHeight="1"/>
     <row r="35" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A35" s="83" t="s">
+      <c r="A35" s="91" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="83"/>
-      <c r="C35" s="83"/>
-      <c r="D35" s="83"/>
-      <c r="E35" s="83"/>
-      <c r="F35" s="83"/>
-      <c r="G35" s="83"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="83"/>
+      <c r="B35" s="91"/>
+      <c r="C35" s="91"/>
+      <c r="D35" s="91"/>
+      <c r="E35" s="91"/>
+      <c r="F35" s="91"/>
+      <c r="G35" s="91"/>
+      <c r="H35" s="91"/>
+      <c r="I35" s="91"/>
     </row>
     <row r="36" spans="1:10" ht="27.95" customHeight="1">
       <c r="A36" s="10" t="s">
@@ -4517,17 +4569,17 @@
       <c r="J48" s="39"/>
     </row>
     <row r="49" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A49" s="83" t="s">
+      <c r="A49" s="91" t="s">
         <v>130</v>
       </c>
-      <c r="B49" s="83"/>
-      <c r="C49" s="83"/>
-      <c r="D49" s="83"/>
-      <c r="E49" s="83"/>
-      <c r="F49" s="83"/>
-      <c r="G49" s="83"/>
-      <c r="H49" s="83"/>
-      <c r="I49" s="84"/>
+      <c r="B49" s="91"/>
+      <c r="C49" s="91"/>
+      <c r="D49" s="91"/>
+      <c r="E49" s="91"/>
+      <c r="F49" s="91"/>
+      <c r="G49" s="91"/>
+      <c r="H49" s="91"/>
+      <c r="I49" s="92"/>
       <c r="J49" s="51"/>
     </row>
     <row r="50" spans="1:10" ht="27.95" customHeight="1">
@@ -5064,17 +5116,17 @@
       </c>
     </row>
     <row r="71" spans="1:9" ht="27.95" customHeight="1">
-      <c r="A71" s="85" t="s">
+      <c r="A71" s="93" t="s">
         <v>145</v>
       </c>
-      <c r="B71" s="85"/>
-      <c r="C71" s="85"/>
-      <c r="D71" s="85"/>
-      <c r="E71" s="85"/>
-      <c r="F71" s="85"/>
-      <c r="G71" s="85"/>
-      <c r="H71" s="85"/>
-      <c r="I71" s="85"/>
+      <c r="B71" s="93"/>
+      <c r="C71" s="93"/>
+      <c r="D71" s="93"/>
+      <c r="E71" s="93"/>
+      <c r="F71" s="93"/>
+      <c r="G71" s="93"/>
+      <c r="H71" s="93"/>
+      <c r="I71" s="93"/>
     </row>
     <row r="72" spans="1:9" ht="27.95" customHeight="1">
       <c r="A72" s="11" t="s">
@@ -5157,7 +5209,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{4D5150BD-60FC-42EC-8538-A0F404D0BC2C}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -5180,7 +5232,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5199,46 +5251,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="106" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="100"/>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
+      <c r="A2" s="108"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="100"/>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
+      <c r="A3" s="108"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="102"/>
-      <c r="B4" s="103"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="103"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
+      <c r="A4" s="110"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="26" t="s">
@@ -5484,90 +5536,90 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" style="116" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="116" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" style="116" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="116" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" style="116" customWidth="1"/>
-    <col min="6" max="6" width="59.5703125" style="116" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" style="116" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="116"/>
+    <col min="1" max="1" width="29.42578125" style="87" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="87" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="87" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="87" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="87" customWidth="1"/>
+    <col min="6" max="6" width="59.5703125" style="87" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" style="87" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="87"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="62.25" customHeight="1">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="112" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="115"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="114"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="115" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="118"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="117"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="C3" s="81" t="s">
         <v>183</v>
       </c>
-      <c r="D3" s="105" t="s">
+      <c r="D3" s="81" t="s">
         <v>184</v>
       </c>
-      <c r="E3" s="105" t="s">
+      <c r="E3" s="81" t="s">
         <v>185</v>
       </c>
-      <c r="F3" s="105" t="s">
+      <c r="F3" s="81" t="s">
         <v>152</v>
       </c>
-      <c r="G3" s="105" t="s">
+      <c r="G3" s="81" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="48" customHeight="1">
-      <c r="A4" s="106" t="s">
+      <c r="A4" s="82" t="s">
         <v>187</v>
       </c>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="C4" s="82" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="107">
+      <c r="D4" s="83">
         <v>45201</v>
       </c>
-      <c r="E4" s="106" t="s">
+      <c r="E4" s="82" t="s">
         <v>189</v>
       </c>
-      <c r="F4" s="106" t="s">
+      <c r="F4" s="82" t="s">
         <v>190</v>
       </c>
-      <c r="G4" s="106"/>
+      <c r="G4" s="82"/>
     </row>
     <row r="5" spans="1:7" ht="48" customHeight="1">
       <c r="A5" s="37" t="s">
@@ -5579,7 +5631,7 @@
       <c r="C5" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="D5" s="108">
+      <c r="D5" s="84">
         <v>45201</v>
       </c>
       <c r="E5" s="37" t="s">
@@ -5600,7 +5652,7 @@
       <c r="C6" s="38" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="109">
+      <c r="D6" s="85">
         <v>45201</v>
       </c>
       <c r="E6" s="38" t="s">
@@ -5612,7 +5664,7 @@
       <c r="G6" s="38"/>
     </row>
     <row r="7" spans="1:7" ht="50.25" customHeight="1">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="86" t="s">
         <v>198</v>
       </c>
       <c r="B7" s="37" t="s">
@@ -5621,7 +5673,7 @@
       <c r="C7" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="D7" s="108">
+      <c r="D7" s="84">
         <v>45201</v>
       </c>
       <c r="E7" s="37" t="s">
@@ -5633,61 +5685,61 @@
       <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="115" t="s">
         <v>201</v>
       </c>
-      <c r="B8" s="111"/>
-      <c r="C8" s="111"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="111"/>
-      <c r="F8" s="111"/>
-      <c r="G8" s="112"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="119"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="105" t="s">
+      <c r="A9" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="105" t="s">
+      <c r="B9" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="105" t="s">
+      <c r="C9" s="81" t="s">
         <v>183</v>
       </c>
-      <c r="D9" s="105" t="s">
+      <c r="D9" s="81" t="s">
         <v>184</v>
       </c>
-      <c r="E9" s="105" t="s">
+      <c r="E9" s="81" t="s">
         <v>185</v>
       </c>
-      <c r="F9" s="105" t="s">
+      <c r="F9" s="81" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="105" t="s">
+      <c r="G9" s="81" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.25">
-      <c r="A10" s="106" t="s">
+    <row r="10" spans="1:7" ht="35.25" customHeight="1">
+      <c r="A10" s="82" t="s">
         <v>202</v>
       </c>
-      <c r="B10" s="106" t="s">
+      <c r="B10" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="106" t="s">
+      <c r="C10" s="82" t="s">
         <v>188</v>
       </c>
-      <c r="D10" s="107">
+      <c r="D10" s="83">
         <v>45208</v>
       </c>
-      <c r="E10" s="106" t="s">
+      <c r="E10" s="82" t="s">
         <v>203</v>
       </c>
-      <c r="F10" s="106" t="s">
+      <c r="F10" s="82" t="s">
         <v>204</v>
       </c>
-      <c r="G10" s="106"/>
-    </row>
-    <row r="11" spans="1:7" ht="33">
+      <c r="G10" s="82"/>
+    </row>
+    <row r="11" spans="1:7" ht="45.75" customHeight="1">
       <c r="A11" s="37" t="s">
         <v>205</v>
       </c>
@@ -5697,7 +5749,7 @@
       <c r="C11" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="D11" s="108">
+      <c r="D11" s="84">
         <v>45208</v>
       </c>
       <c r="E11" s="37" t="s">
@@ -5710,7 +5762,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="33">
+    <row r="12" spans="1:7" ht="39" customHeight="1">
       <c r="A12" s="38" t="s">
         <v>208</v>
       </c>
@@ -5720,7 +5772,7 @@
       <c r="C12" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="D12" s="109">
+      <c r="D12" s="85">
         <v>45208</v>
       </c>
       <c r="E12" s="38" t="s">
@@ -5731,8 +5783,8 @@
       </c>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:7" ht="17.25">
-      <c r="A13" s="110" t="s">
+    <row r="13" spans="1:7" ht="39.75" customHeight="1">
+      <c r="A13" s="86" t="s">
         <v>211</v>
       </c>
       <c r="B13" s="37" t="s">
@@ -5741,7 +5793,7 @@
       <c r="C13" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D13" s="108">
+      <c r="D13" s="84">
         <v>45208</v>
       </c>
       <c r="E13" s="37" t="s">
@@ -5753,156 +5805,320 @@
       <c r="G13" s="37"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="104" t="s">
+      <c r="A14" s="115" t="s">
         <v>214</v>
       </c>
-      <c r="B14" s="111"/>
-      <c r="C14" s="111"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="111"/>
-      <c r="G14" s="112"/>
+      <c r="B14" s="118"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="118"/>
+      <c r="G14" s="119"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="105" t="s">
+      <c r="A15" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="B15" s="105" t="s">
+      <c r="B15" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="105" t="s">
+      <c r="C15" s="81" t="s">
         <v>183</v>
       </c>
-      <c r="D15" s="105" t="s">
+      <c r="D15" s="81" t="s">
         <v>184</v>
       </c>
-      <c r="E15" s="105" t="s">
+      <c r="E15" s="81" t="s">
         <v>185</v>
       </c>
-      <c r="F15" s="105" t="s">
+      <c r="F15" s="81" t="s">
         <v>152</v>
       </c>
-      <c r="G15" s="105" t="s">
+      <c r="G15" s="81" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="33">
-      <c r="A16" s="106" t="s">
+    <row r="16" spans="1:7" ht="38.25" customHeight="1">
+      <c r="A16" s="82" t="s">
         <v>215</v>
       </c>
-      <c r="B16" s="106" t="s">
+      <c r="B16" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="C16" s="107" t="s">
+      <c r="C16" s="83" t="s">
         <v>188</v>
       </c>
-      <c r="D16" s="107">
+      <c r="D16" s="83">
         <v>45212</v>
       </c>
-      <c r="E16" s="106" t="s">
+      <c r="E16" s="82" t="s">
         <v>203</v>
       </c>
-      <c r="G16" s="106"/>
-    </row>
-    <row r="17" spans="1:7" ht="17.25">
+      <c r="F16" s="82" t="s">
+        <v>222</v>
+      </c>
+      <c r="G16" s="82"/>
+    </row>
+    <row r="17" spans="1:7" ht="27" customHeight="1">
       <c r="A17" s="37" t="s">
         <v>216</v>
       </c>
       <c r="B17" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="C17" s="108" t="s">
+      <c r="C17" s="84" t="s">
         <v>188</v>
       </c>
-      <c r="D17" s="108">
+      <c r="D17" s="84">
         <v>45212</v>
       </c>
       <c r="E17" s="37" t="s">
         <v>199</v>
       </c>
+      <c r="F17" s="37" t="s">
+        <v>223</v>
+      </c>
       <c r="G17" s="37"/>
     </row>
-    <row r="18" spans="1:7" ht="17.25">
+    <row r="18" spans="1:7" ht="24" customHeight="1">
       <c r="A18" s="38" t="s">
         <v>205</v>
       </c>
       <c r="B18" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="C18" s="107" t="s">
+      <c r="C18" s="83" t="s">
         <v>188</v>
       </c>
-      <c r="D18" s="109">
+      <c r="D18" s="85">
         <v>45212</v>
       </c>
       <c r="E18" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="F18" s="119"/>
-      <c r="G18" s="106" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="17.25">
-      <c r="A19" s="110" t="s">
+      <c r="F18" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="G18" s="82"/>
+    </row>
+    <row r="19" spans="1:7" ht="40.5" customHeight="1">
+      <c r="A19" s="86" t="s">
         <v>217</v>
       </c>
       <c r="B19" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="108" t="s">
+      <c r="C19" s="84" t="s">
         <v>188</v>
       </c>
-      <c r="D19" s="108">
+      <c r="D19" s="84">
         <v>45212</v>
       </c>
       <c r="E19" s="37" t="s">
         <v>218</v>
       </c>
+      <c r="F19" s="37" t="s">
+        <v>225</v>
+      </c>
       <c r="G19" s="37"/>
     </row>
-    <row r="20" spans="1:7" ht="17.25">
+    <row r="20" spans="1:7" ht="26.25" customHeight="1">
       <c r="A20" s="38" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="C20" s="107" t="s">
+      <c r="C20" s="83" t="s">
         <v>188</v>
       </c>
-      <c r="D20" s="109">
+      <c r="D20" s="85">
         <v>45212</v>
       </c>
       <c r="E20" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="G20" s="82"/>
+    </row>
+    <row r="21" spans="1:7" ht="46.5" customHeight="1">
+      <c r="A21" s="86" t="s">
         <v>220</v>
-      </c>
-      <c r="G20" s="106"/>
-    </row>
-    <row r="21" spans="1:7" ht="33">
-      <c r="A21" s="110" t="s">
-        <v>221</v>
       </c>
       <c r="B21" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="108" t="s">
+      <c r="C21" s="84" t="s">
         <v>188</v>
       </c>
-      <c r="D21" s="108">
+      <c r="D21" s="84">
         <v>45212</v>
       </c>
       <c r="E21" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="G21" s="37"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="115" t="s">
+        <v>229</v>
+      </c>
+      <c r="B22" s="118"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="118"/>
+      <c r="G22" s="119"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="81" t="s">
+        <v>182</v>
+      </c>
+      <c r="B23" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="81" t="s">
+        <v>183</v>
+      </c>
+      <c r="D23" s="81" t="s">
+        <v>184</v>
+      </c>
+      <c r="E23" s="81" t="s">
+        <v>185</v>
+      </c>
+      <c r="F23" s="81" t="s">
+        <v>152</v>
+      </c>
+      <c r="G23" s="81" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A24" s="82" t="s">
+        <v>230</v>
+      </c>
+      <c r="B24" s="82" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="83" t="s">
+        <v>188</v>
+      </c>
+      <c r="D24" s="83">
+        <v>45222</v>
+      </c>
+      <c r="E24" s="82" t="s">
+        <v>203</v>
+      </c>
+      <c r="F24" s="82" t="s">
         <v>222</v>
       </c>
-      <c r="G21" s="37"/>
+      <c r="G24" s="82"/>
+    </row>
+    <row r="25" spans="1:7" ht="34.5" customHeight="1">
+      <c r="A25" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="84" t="s">
+        <v>188</v>
+      </c>
+      <c r="D25" s="84">
+        <v>45222</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="G25" s="37"/>
+    </row>
+    <row r="26" spans="1:7" ht="34.5" customHeight="1">
+      <c r="A26" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="83" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" s="85">
+        <v>45222</v>
+      </c>
+      <c r="E26" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="F26" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="G26" s="82"/>
+    </row>
+    <row r="27" spans="1:7" ht="33" customHeight="1">
+      <c r="A27" s="86" t="s">
+        <v>233</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="84" t="s">
+        <v>188</v>
+      </c>
+      <c r="D27" s="84">
+        <v>45222</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="G27" s="37"/>
+    </row>
+    <row r="28" spans="1:7" ht="28.5" customHeight="1">
+      <c r="A28" s="120" t="s">
+        <v>234</v>
+      </c>
+      <c r="B28" s="120" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="121" t="s">
+        <v>188</v>
+      </c>
+      <c r="D28" s="121">
+        <v>45222</v>
+      </c>
+      <c r="E28" s="120" t="s">
+        <v>219</v>
+      </c>
+      <c r="F28" s="120" t="s">
+        <v>227</v>
+      </c>
+      <c r="G28" s="120"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="88"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="88"/>
+      <c r="G29" s="88"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A22:G22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajustes site e documentação
</commit_message>
<xml_diff>
--- a/Documentação/backLogs e Planos de ação/planoDeAção BackLog PlanilhaDeRiscos.xlsx
+++ b/Documentação/backLogs e Planos de ação/planoDeAção BackLog PlanilhaDeRiscos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="BackLogs" sheetId="4" r:id="rId1"/>
@@ -17,49 +17,17 @@
     <sheet name="Plano de Ação" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="236">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -766,6 +734,9 @@
   </si>
   <si>
     <t xml:space="preserve">Modulo analytics </t>
+  </si>
+  <si>
+    <t>Descrição de arquitetura técnica e simplificada para o técnico de TI e usuário</t>
   </si>
 </sst>
 </file>
@@ -3104,8 +3075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27.95" customHeight="1"/>
@@ -3341,57 +3312,57 @@
 )</f>
         <v>163</v>
       </c>
-      <c r="N4" s="67" cm="1">
+      <c r="N4" s="67">
         <f t="array" ref="N4">IF(SUM(N3)&gt;0,M4-N3,n
 )</f>
         <v>147</v>
       </c>
-      <c r="O4" s="67" cm="1">
+      <c r="O4" s="67">
         <f t="array" ref="O4">IF(SUM(O3)&gt;0,N4-O3,n
 )</f>
         <v>130</v>
       </c>
-      <c r="P4" s="67" cm="1">
+      <c r="P4" s="67">
         <f t="array" ref="P4">IF(SUM(P3)&gt;0,O4-P3,n
 )</f>
         <v>112</v>
       </c>
-      <c r="Q4" s="67" cm="1">
+      <c r="Q4" s="67">
         <f t="array" ref="Q4">IF(SUM(Q3)&gt;0,P4-Q3,n
 )</f>
         <v>95</v>
       </c>
-      <c r="R4" s="67" cm="1">
+      <c r="R4" s="67">
         <f t="array" ref="R4">IF(SUM(R3)&gt;0,Q4-R3,n
 )</f>
         <v>80</v>
       </c>
-      <c r="S4" s="67" cm="1">
+      <c r="S4" s="67">
         <f t="array" ref="S4">IF(SUM(S3)&gt;0,R4-S3,n
 )</f>
         <v>64</v>
       </c>
-      <c r="T4" s="67" cm="1">
+      <c r="T4" s="67">
         <f t="array" ref="T4">IF(SUM(T3)&gt;0,S4-T3,n
 )</f>
         <v>47</v>
       </c>
-      <c r="U4" s="67" cm="1">
+      <c r="U4" s="67">
         <f t="array" ref="U4">IF(SUM(U3)&gt;0,T4-U3,n
 )</f>
         <v>31</v>
       </c>
-      <c r="V4" s="67" cm="1">
+      <c r="V4" s="67">
         <f t="array" ref="V4">IF(SUM(V3)&gt;0,U4-V3,n
 )</f>
         <v>16</v>
       </c>
-      <c r="W4" s="67" cm="1">
+      <c r="W4" s="67">
         <f t="array" ref="W4">IF(SUM(W3)&gt;0,V4-W3,n
 )</f>
         <v>0</v>
       </c>
-      <c r="X4" s="67" t="e" cm="1">
+      <c r="X4" s="67" t="e">
         <f t="array" ref="X4">IF(SUM(X3)&gt;0,W4-X3,n
 )</f>
         <v>#NAME?</v>
@@ -3664,7 +3635,7 @@
         <v>68</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>44</v>
@@ -5210,7 +5181,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="gap">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -5236,8 +5207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScale="145" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
foram adicionados requisitos da sprint 3
</commit_message>
<xml_diff>
--- a/Documentação/backLogs e Planos de ação/planoDeAção BackLog PlanilhaDeRiscos.xlsx
+++ b/Documentação/backLogs e Planos de ação/planoDeAção BackLog PlanilhaDeRiscos.xlsx
@@ -1,33 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Desktop\Material Sptech\Projetos\MushRoomCompany\Documentação\backLogs e Planos de ação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pehso\Downloads\git backaup\MushRoomCompany\Documentação\backLogs e Planos de ação\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710717FF-96A9-4CC9-84F5-914818D8194F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLogs" sheetId="4" r:id="rId1"/>
     <sheet name="Planilha de Riscos" sheetId="2" r:id="rId2"/>
     <sheet name="Plano de Ação" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="245">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -737,16 +748,43 @@
   </si>
   <si>
     <t>Descrição de arquitetura técnica e simplificada para o técnico de TI e usuário</t>
+  </si>
+  <si>
+    <t>• Manual de Instalação</t>
+  </si>
+  <si>
+    <t>Planilha de Homologação do Projeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluxograma do suporte </t>
+  </si>
+  <si>
+    <t>Ferramenta de Help Desk</t>
+  </si>
+  <si>
+    <t>Documento de Mudança</t>
+  </si>
+  <si>
+    <t>Integração com o banco de dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teste integrado do analytics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teste integrado da solução de IoT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagrama de fácil  visualização para o cliente e que apresente uma visão geral do funcionamento do projeto. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -872,6 +910,18 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Quire Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1368,7 +1418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1631,107 +1681,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="31" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="31" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1909,7 +1971,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3072,17 +3133,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="27.95" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="104.7109375" style="7" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" style="7" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" style="7" customWidth="1"/>
@@ -3106,35 +3167,35 @@
     <col min="25" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="53.25" customHeight="1">
+    <row r="1" spans="1:24" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="98"/>
-      <c r="L1" s="91" t="s">
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="97"/>
+      <c r="L1" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="92"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="92"/>
-      <c r="W1" s="92"/>
-      <c r="X1" s="92"/>
-    </row>
-    <row r="2" spans="1:24" ht="27.95" customHeight="1">
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91"/>
+      <c r="X1" s="91"/>
+    </row>
+    <row r="2" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -3202,7 +3263,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="27.95" customHeight="1">
+    <row r="3" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
@@ -3272,7 +3333,7 @@
       </c>
       <c r="X3" s="66"/>
     </row>
-    <row r="4" spans="1:24" ht="27.95" customHeight="1">
+    <row r="4" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>32</v>
       </c>
@@ -3368,7 +3429,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="27.95" customHeight="1">
+    <row r="5" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>36</v>
       </c>
@@ -3410,7 +3471,7 @@
       <c r="W5" s="70"/>
       <c r="X5" s="70"/>
     </row>
-    <row r="6" spans="1:24" ht="27.95" customHeight="1">
+    <row r="6" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>41</v>
       </c>
@@ -3439,47 +3500,47 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="27.95" customHeight="1">
-      <c r="A7" s="104" t="s">
+    <row r="7" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="101" t="s">
+      <c r="C7" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="102" t="s">
+      <c r="D7" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="103" t="s">
+      <c r="E7" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="100" t="s">
+      <c r="F7" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="100">
+      <c r="G7" s="99">
         <v>8</v>
       </c>
-      <c r="H7" s="99">
+      <c r="H7" s="98">
         <v>4</v>
       </c>
-      <c r="I7" s="106" t="s">
+      <c r="I7" s="105" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="27.95" customHeight="1">
-      <c r="A8" s="105"/>
-      <c r="B8" s="101"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="100"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="107"/>
-    </row>
-    <row r="9" spans="1:24" ht="27.95" customHeight="1">
+    <row r="8" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="104"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="99"/>
+      <c r="G8" s="99"/>
+      <c r="H8" s="98"/>
+      <c r="I8" s="106"/>
+    </row>
+    <row r="9" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>50</v>
       </c>
@@ -3508,7 +3569,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="27.95" customHeight="1">
+    <row r="10" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>53</v>
       </c>
@@ -3540,7 +3601,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="27.95" customHeight="1">
+    <row r="11" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>57</v>
       </c>
@@ -3569,7 +3630,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="27.95" customHeight="1">
+    <row r="12" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>61</v>
       </c>
@@ -3598,7 +3659,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="27.95" customHeight="1">
+    <row r="13" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>64</v>
       </c>
@@ -3627,7 +3688,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="27.95" customHeight="1">
+    <row r="14" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>67</v>
       </c>
@@ -3656,7 +3717,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="27.95" customHeight="1">
+    <row r="15" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>71</v>
       </c>
@@ -3685,7 +3746,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="27.95" customHeight="1">
+    <row r="16" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>74</v>
       </c>
@@ -3714,7 +3775,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="27.95" customHeight="1">
+    <row r="17" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>77</v>
       </c>
@@ -3743,7 +3804,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="26.25" customHeight="1">
+    <row r="18" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>80</v>
       </c>
@@ -3772,7 +3833,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="27.95" customHeight="1">
+    <row r="19" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>83</v>
       </c>
@@ -3801,7 +3862,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="27.95" customHeight="1">
+    <row r="20" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>86</v>
       </c>
@@ -3830,7 +3891,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="27.95" customHeight="1">
+    <row r="21" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>89</v>
       </c>
@@ -3859,7 +3920,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="27.95" customHeight="1">
+    <row r="22" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>92</v>
       </c>
@@ -3888,7 +3949,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="27.95" customHeight="1">
+    <row r="23" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>96</v>
       </c>
@@ -3917,7 +3978,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="27.95" customHeight="1">
+    <row r="24" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>99</v>
       </c>
@@ -3946,7 +4007,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="27.95" customHeight="1">
+    <row r="25" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>103</v>
       </c>
@@ -3975,7 +4036,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="27.95" customHeight="1">
+    <row r="26" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="76" t="s">
         <v>106</v>
       </c>
@@ -4002,7 +4063,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="27.95" customHeight="1">
+    <row r="27" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>109</v>
       </c>
@@ -4029,7 +4090,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="27.95" customHeight="1">
+    <row r="28" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>112</v>
       </c>
@@ -4056,7 +4117,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="27.95" customHeight="1">
+    <row r="29" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>115</v>
       </c>
@@ -4083,7 +4144,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="27.95" customHeight="1">
+    <row r="30" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>118</v>
       </c>
@@ -4110,7 +4171,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="27.95" customHeight="1">
+    <row r="31" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>121</v>
       </c>
@@ -4137,7 +4198,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="27.95" customHeight="1">
+    <row r="32" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>124</v>
       </c>
@@ -4164,7 +4225,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="24" customHeight="1">
+    <row r="33" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>127</v>
       </c>
@@ -4191,21 +4252,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="30.75" customHeight="1"/>
-    <row r="35" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A35" s="93" t="s">
+    <row r="34" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="92" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="93"/>
-      <c r="C35" s="93"/>
-      <c r="D35" s="93"/>
-      <c r="E35" s="93"/>
-      <c r="F35" s="93"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="93"/>
-    </row>
-    <row r="36" spans="1:10" ht="27.95" customHeight="1">
+      <c r="B35" s="92"/>
+      <c r="C35" s="92"/>
+      <c r="D35" s="92"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="92"/>
+      <c r="G35" s="92"/>
+      <c r="H35" s="92"/>
+      <c r="I35" s="92"/>
+    </row>
+    <row r="36" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>36</v>
       </c>
@@ -4234,7 +4295,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="27.95" customHeight="1">
+    <row r="37" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>50</v>
       </c>
@@ -4263,7 +4324,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="27.95" customHeight="1">
+    <row r="38" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>61</v>
       </c>
@@ -4292,7 +4353,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="27.95" customHeight="1">
+    <row r="39" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>77</v>
       </c>
@@ -4321,7 +4382,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="27.75" customHeight="1">
+    <row r="40" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>106</v>
       </c>
@@ -4348,7 +4409,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="45.75" hidden="1" customHeight="1">
+    <row r="41" spans="1:10" ht="45.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>109</v>
       </c>
@@ -4375,7 +4436,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="45.75" customHeight="1">
+    <row r="42" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>112</v>
       </c>
@@ -4402,7 +4463,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="27.95" customHeight="1">
+    <row r="43" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>115</v>
       </c>
@@ -4429,7 +4490,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="27.95" customHeight="1">
+    <row r="44" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>118</v>
       </c>
@@ -4456,7 +4517,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="27.95" customHeight="1">
+    <row r="45" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>121</v>
       </c>
@@ -4483,7 +4544,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="27.95" customHeight="1">
+    <row r="46" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>124</v>
       </c>
@@ -4510,7 +4571,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="27.95" customHeight="1">
+    <row r="47" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>127</v>
       </c>
@@ -4537,24 +4598,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="27.95" customHeight="1">
+    <row r="48" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J48" s="39"/>
     </row>
-    <row r="49" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A49" s="93" t="s">
+    <row r="49" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="92" t="s">
         <v>130</v>
       </c>
-      <c r="B49" s="93"/>
-      <c r="C49" s="93"/>
-      <c r="D49" s="93"/>
-      <c r="E49" s="93"/>
-      <c r="F49" s="93"/>
-      <c r="G49" s="93"/>
-      <c r="H49" s="93"/>
-      <c r="I49" s="94"/>
+      <c r="B49" s="92"/>
+      <c r="C49" s="92"/>
+      <c r="D49" s="92"/>
+      <c r="E49" s="92"/>
+      <c r="F49" s="92"/>
+      <c r="G49" s="92"/>
+      <c r="H49" s="92"/>
+      <c r="I49" s="93"/>
       <c r="J49" s="51"/>
     </row>
-    <row r="50" spans="1:10" ht="27.95" customHeight="1">
+    <row r="50" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="43" t="s">
         <v>24</v>
       </c>
@@ -4583,7 +4644,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="27.95" customHeight="1">
+    <row r="51" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="43" t="s">
         <v>32</v>
       </c>
@@ -4612,7 +4673,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="27.95" customHeight="1">
+    <row r="52" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="47" t="s">
         <v>41</v>
       </c>
@@ -4641,7 +4702,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="27.95" customHeight="1">
+    <row r="53" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="64" t="s">
         <v>47</v>
       </c>
@@ -4670,7 +4731,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="27.95" customHeight="1">
+    <row r="54" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="65"/>
       <c r="B54" s="55"/>
       <c r="C54" s="55"/>
@@ -4681,7 +4742,7 @@
       <c r="H54" s="59"/>
       <c r="I54" s="57"/>
     </row>
-    <row r="55" spans="1:10" ht="27.95" customHeight="1">
+    <row r="55" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="43" t="s">
         <v>64</v>
       </c>
@@ -4710,7 +4771,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="27.95" customHeight="1">
+    <row r="56" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="47" t="s">
         <v>57</v>
       </c>
@@ -4739,7 +4800,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="27.95" customHeight="1">
+    <row r="57" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="43" t="s">
         <v>74</v>
       </c>
@@ -4768,7 +4829,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="27.95" customHeight="1">
+    <row r="58" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="43" t="s">
         <v>80</v>
       </c>
@@ -4797,7 +4858,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="27.95" customHeight="1">
+    <row r="59" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="43" t="s">
         <v>83</v>
       </c>
@@ -4826,7 +4887,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="27.95" customHeight="1">
+    <row r="60" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="43" t="s">
         <v>86</v>
       </c>
@@ -4855,7 +4916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="27.95" customHeight="1">
+    <row r="61" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="47" t="s">
         <v>71</v>
       </c>
@@ -4884,7 +4945,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="27.95" customHeight="1">
+    <row r="62" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="43" t="s">
         <v>80</v>
       </c>
@@ -4913,7 +4974,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="27.95" customHeight="1">
+    <row r="63" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="43" t="s">
         <v>118</v>
       </c>
@@ -4942,7 +5003,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="27.95" customHeight="1">
+    <row r="64" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="43" t="s">
         <v>83</v>
       </c>
@@ -4971,7 +5032,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="27.95" customHeight="1">
+    <row r="65" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="47" t="s">
         <v>89</v>
       </c>
@@ -5000,7 +5061,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="27.95" customHeight="1">
+    <row r="66" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="43" t="s">
         <v>142</v>
       </c>
@@ -5029,7 +5090,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="27.95" customHeight="1">
+    <row r="67" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="43" t="s">
         <v>143</v>
       </c>
@@ -5058,7 +5119,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="27.95" customHeight="1">
+    <row r="68" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="43" t="s">
         <v>144</v>
       </c>
@@ -5087,20 +5148,20 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="27.95" customHeight="1">
-      <c r="A71" s="95" t="s">
+    <row r="71" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="94" t="s">
         <v>145</v>
       </c>
-      <c r="B71" s="95"/>
-      <c r="C71" s="95"/>
-      <c r="D71" s="95"/>
-      <c r="E71" s="95"/>
-      <c r="F71" s="95"/>
-      <c r="G71" s="95"/>
-      <c r="H71" s="95"/>
-      <c r="I71" s="95"/>
-    </row>
-    <row r="72" spans="1:9" ht="27.95" customHeight="1">
+      <c r="B71" s="94"/>
+      <c r="C71" s="94"/>
+      <c r="D71" s="94"/>
+      <c r="E71" s="94"/>
+      <c r="F71" s="94"/>
+      <c r="G71" s="94"/>
+      <c r="H71" s="94"/>
+      <c r="I71" s="94"/>
+    </row>
+    <row r="72" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>67</v>
       </c>
@@ -5108,7 +5169,7 @@
         <v>68</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>69</v>
+        <v>244</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>44</v>
@@ -5129,7 +5190,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="27.95" customHeight="1">
+    <row r="73" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>80</v>
       </c>
@@ -5157,6 +5218,145 @@
       <c r="I73" s="22" t="s">
         <v>70</v>
       </c>
+    </row>
+    <row r="74" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B74" s="123" t="s">
+        <v>236</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
+    </row>
+    <row r="75" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75" s="123" t="s">
+        <v>237</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
+    </row>
+    <row r="76" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="121" t="s">
+        <v>96</v>
+      </c>
+      <c r="B76" s="124" t="s">
+        <v>238</v>
+      </c>
+      <c r="C76" s="122" t="s">
+        <v>69</v>
+      </c>
+      <c r="D76" s="122"/>
+      <c r="E76" s="122"/>
+      <c r="F76" s="122"/>
+      <c r="G76" s="122"/>
+      <c r="H76" s="122"/>
+      <c r="I76" s="122"/>
+    </row>
+    <row r="77" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77" s="123" t="s">
+        <v>239</v>
+      </c>
+      <c r="C77" s="122" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+    </row>
+    <row r="78" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B78" s="123" t="s">
+        <v>240</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+    </row>
+    <row r="79" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+    </row>
+    <row r="80" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B80" s="123" t="s">
+        <v>242</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+    </row>
+    <row r="81" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B81" s="123" t="s">
+        <v>243</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+    </row>
+    <row r="84" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -5175,13 +5375,14 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="I7:I8"/>
   </mergeCells>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="gap">
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="gap" xr2:uid="{00000000-0003-0000-0000-000000000000}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -5204,14 +5405,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView zoomScale="145" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
@@ -5222,49 +5423,49 @@
     <col min="8" max="8" width="67" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="108" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="107" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="110"/>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="110"/>
-      <c r="B3" s="111"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="112"/>
-      <c r="B4" s="113"/>
-      <c r="C4" s="113"/>
-      <c r="D4" s="113"/>
-      <c r="E4" s="113"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="113"/>
-      <c r="H4" s="113"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="109"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="109"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="110"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="111"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>147</v>
       </c>
@@ -5290,7 +5491,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>1</v>
       </c>
@@ -5316,7 +5517,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <v>2</v>
       </c>
@@ -5342,7 +5543,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>3</v>
       </c>
@@ -5368,7 +5569,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>4</v>
       </c>
@@ -5394,7 +5595,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="11.25" customHeight="1">
+    <row r="10" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>5</v>
       </c>
@@ -5420,7 +5621,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>6</v>
       </c>
@@ -5446,7 +5647,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>7</v>
       </c>
@@ -5472,7 +5673,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>8</v>
       </c>
@@ -5498,7 +5699,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" ht="11.25" customHeight="1"/>
+    <row r="17" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H4"/>
@@ -5508,14 +5709,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView zoomScale="81" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" style="87" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" style="87" customWidth="1"/>
@@ -5527,29 +5728,29 @@
     <col min="8" max="16384" width="9.140625" style="87"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="62.25" customHeight="1">
-      <c r="A1" s="114" t="s">
+    <row r="1" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="113" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="116"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="117" t="s">
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="115"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="116" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="119"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="118"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="81" t="s">
         <v>182</v>
       </c>
@@ -5572,7 +5773,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="48" customHeight="1">
+    <row r="4" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="82" t="s">
         <v>187</v>
       </c>
@@ -5593,7 +5794,7 @@
       </c>
       <c r="G4" s="82"/>
     </row>
-    <row r="5" spans="1:7" ht="48" customHeight="1">
+    <row r="5" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
         <v>191</v>
       </c>
@@ -5614,7 +5815,7 @@
       </c>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" spans="1:7" ht="48" customHeight="1">
+    <row r="6" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>195</v>
       </c>
@@ -5635,7 +5836,7 @@
       </c>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7" ht="50.25" customHeight="1">
+    <row r="7" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="86" t="s">
         <v>198</v>
       </c>
@@ -5656,18 +5857,18 @@
       </c>
       <c r="G7" s="37"/>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="117" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="116" t="s">
         <v>201</v>
       </c>
-      <c r="B8" s="120"/>
-      <c r="C8" s="120"/>
-      <c r="D8" s="120"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="120"/>
-      <c r="G8" s="121"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="B8" s="119"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="119"/>
+      <c r="G8" s="120"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="81" t="s">
         <v>182</v>
       </c>
@@ -5690,7 +5891,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="35.25" customHeight="1">
+    <row r="10" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="82" t="s">
         <v>202</v>
       </c>
@@ -5711,7 +5912,7 @@
       </c>
       <c r="G10" s="82"/>
     </row>
-    <row r="11" spans="1:7" ht="45.75" customHeight="1">
+    <row r="11" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
         <v>205</v>
       </c>
@@ -5734,7 +5935,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="39" customHeight="1">
+    <row r="12" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
         <v>208</v>
       </c>
@@ -5755,7 +5956,7 @@
       </c>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:7" ht="39.75" customHeight="1">
+    <row r="13" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="86" t="s">
         <v>211</v>
       </c>
@@ -5776,18 +5977,18 @@
       </c>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="117" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="116" t="s">
         <v>214</v>
       </c>
-      <c r="B14" s="120"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="121"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="B14" s="119"/>
+      <c r="C14" s="119"/>
+      <c r="D14" s="119"/>
+      <c r="E14" s="119"/>
+      <c r="F14" s="119"/>
+      <c r="G14" s="120"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="81" t="s">
         <v>182</v>
       </c>
@@ -5810,7 +6011,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="38.25" customHeight="1">
+    <row r="16" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="82" t="s">
         <v>215</v>
       </c>
@@ -5831,7 +6032,7 @@
       </c>
       <c r="G16" s="82"/>
     </row>
-    <row r="17" spans="1:7" ht="27" customHeight="1">
+    <row r="17" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>216</v>
       </c>
@@ -5852,7 +6053,7 @@
       </c>
       <c r="G17" s="37"/>
     </row>
-    <row r="18" spans="1:7" ht="24" customHeight="1">
+    <row r="18" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>205</v>
       </c>
@@ -5873,7 +6074,7 @@
       </c>
       <c r="G18" s="82"/>
     </row>
-    <row r="19" spans="1:7" ht="40.5" customHeight="1">
+    <row r="19" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="86" t="s">
         <v>217</v>
       </c>
@@ -5894,7 +6095,7 @@
       </c>
       <c r="G19" s="37"/>
     </row>
-    <row r="20" spans="1:7" ht="26.25" customHeight="1">
+    <row r="20" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
         <v>226</v>
       </c>
@@ -5915,7 +6116,7 @@
       </c>
       <c r="G20" s="82"/>
     </row>
-    <row r="21" spans="1:7" ht="46.5" customHeight="1">
+    <row r="21" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="86" t="s">
         <v>220</v>
       </c>
@@ -5936,18 +6137,18 @@
       </c>
       <c r="G21" s="37"/>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="117" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="116" t="s">
         <v>229</v>
       </c>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-      <c r="G22" s="121"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="B22" s="119"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="119"/>
+      <c r="G22" s="120"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="81" t="s">
         <v>182</v>
       </c>
@@ -5970,7 +6171,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="26.25" customHeight="1">
+    <row r="24" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="82" t="s">
         <v>230</v>
       </c>
@@ -5991,7 +6192,7 @@
       </c>
       <c r="G24" s="82"/>
     </row>
-    <row r="25" spans="1:7" ht="34.5" customHeight="1">
+    <row r="25" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
         <v>231</v>
       </c>
@@ -6012,7 +6213,7 @@
       </c>
       <c r="G25" s="37"/>
     </row>
-    <row r="26" spans="1:7" ht="34.5" customHeight="1">
+    <row r="26" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="38" t="s">
         <v>232</v>
       </c>
@@ -6033,7 +6234,7 @@
       </c>
       <c r="G26" s="82"/>
     </row>
-    <row r="27" spans="1:7" ht="33" customHeight="1">
+    <row r="27" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="86" t="s">
         <v>233</v>
       </c>
@@ -6054,35 +6255,26 @@
       </c>
       <c r="G27" s="37"/>
     </row>
-    <row r="28" spans="1:7" ht="28.5" customHeight="1">
-      <c r="A28" s="89" t="s">
+    <row r="28" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="88" t="s">
         <v>234</v>
       </c>
-      <c r="B28" s="89" t="s">
+      <c r="B28" s="88" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="90" t="s">
+      <c r="C28" s="89" t="s">
         <v>188</v>
       </c>
-      <c r="D28" s="90">
+      <c r="D28" s="89">
         <v>45222</v>
       </c>
-      <c r="E28" s="89" t="s">
+      <c r="E28" s="88" t="s">
         <v>219</v>
       </c>
-      <c r="F28" s="89" t="s">
+      <c r="F28" s="88" t="s">
         <v>227</v>
       </c>
-      <c r="G28" s="89"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="88"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="88"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="88"/>
+      <c r="G28" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Atualizaçao backlog de requisitos
</commit_message>
<xml_diff>
--- a/Documentação/backLogs e Planos de ação/planoDeAção BackLog PlanilhaDeRiscos.xlsx
+++ b/Documentação/backLogs e Planos de ação/planoDeAção BackLog PlanilhaDeRiscos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pehso\Downloads\git backaup\MushRoomCompany\Documentação\backLogs e Planos de ação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710717FF-96A9-4CC9-84F5-914818D8194F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7757BA-1B6D-48E1-BA1A-E6350EE4481C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLogs" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="250">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -775,6 +775,21 @@
   </si>
   <si>
     <t xml:space="preserve">Diagrama de fácil  visualização para o cliente e que apresente uma visão geral do funcionamento do projeto. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual com instruções e passo a passo de monntagem do ardoino </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fluxograma visual do funcionamento dos chamados de suporte </t>
+  </si>
+  <si>
+    <t>ferramenta para abrir chamados de incidentes, problemas e requisições</t>
+  </si>
+  <si>
+    <t>formulario de gmud</t>
+  </si>
+  <si>
+    <t>Inportante</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1687,6 +1702,18 @@
     <xf numFmtId="164" fontId="8" fillId="31" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1779,21 +1806,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3134,68 +3146,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X84"/>
+  <dimension ref="A1:X81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="27.9" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="104.7109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="7"/>
-    <col min="11" max="11" width="31.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="15.85546875" style="7" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="7"/>
+    <col min="11" max="11" width="31.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="15.88671875" style="7" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="16.44140625" style="7" customWidth="1"/>
     <col min="17" max="17" width="16" style="7" customWidth="1"/>
-    <col min="18" max="19" width="15.7109375" style="7" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" style="7" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" style="7" customWidth="1"/>
-    <col min="22" max="22" width="16.28515625" style="7" customWidth="1"/>
-    <col min="23" max="23" width="16.7109375" style="7" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" style="7" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="7"/>
+    <col min="18" max="19" width="15.6640625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="15.88671875" style="7" customWidth="1"/>
+    <col min="21" max="21" width="16.109375" style="7" customWidth="1"/>
+    <col min="22" max="22" width="16.33203125" style="7" customWidth="1"/>
+    <col min="23" max="23" width="16.6640625" style="7" customWidth="1"/>
+    <col min="24" max="24" width="15.88671875" style="7" customWidth="1"/>
+    <col min="25" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="97"/>
-      <c r="L1" s="90" t="s">
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="101"/>
+      <c r="L1" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91"/>
-      <c r="S1" s="91"/>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91"/>
-      <c r="X1" s="91"/>
-    </row>
-    <row r="2" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="95"/>
+      <c r="P1" s="95"/>
+      <c r="Q1" s="95"/>
+      <c r="R1" s="95"/>
+      <c r="S1" s="95"/>
+      <c r="T1" s="95"/>
+      <c r="U1" s="95"/>
+      <c r="V1" s="95"/>
+      <c r="W1" s="95"/>
+      <c r="X1" s="95"/>
+    </row>
+    <row r="2" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -3263,7 +3275,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
@@ -3333,7 +3345,7 @@
       </c>
       <c r="X3" s="66"/>
     </row>
-    <row r="4" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>32</v>
       </c>
@@ -3429,7 +3441,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>36</v>
       </c>
@@ -3471,7 +3483,7 @@
       <c r="W5" s="70"/>
       <c r="X5" s="70"/>
     </row>
-    <row r="6" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>41</v>
       </c>
@@ -3500,47 +3512,47 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+    <row r="7" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="107" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="B7" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="100" t="s">
+      <c r="C7" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="101" t="s">
+      <c r="D7" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="102" t="s">
+      <c r="E7" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="99" t="s">
+      <c r="F7" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="99">
+      <c r="G7" s="103">
         <v>8</v>
       </c>
-      <c r="H7" s="98">
+      <c r="H7" s="102">
         <v>4</v>
       </c>
-      <c r="I7" s="105" t="s">
+      <c r="I7" s="109" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="104"/>
-      <c r="B8" s="100"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="106"/>
-    </row>
-    <row r="9" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="108"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="106"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="110"/>
+    </row>
+    <row r="9" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>50</v>
       </c>
@@ -3569,7 +3581,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>53</v>
       </c>
@@ -3601,7 +3613,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>57</v>
       </c>
@@ -3630,7 +3642,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>61</v>
       </c>
@@ -3659,7 +3671,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>64</v>
       </c>
@@ -3688,7 +3700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>67</v>
       </c>
@@ -3717,7 +3729,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>71</v>
       </c>
@@ -3746,7 +3758,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>74</v>
       </c>
@@ -3775,7 +3787,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>77</v>
       </c>
@@ -3804,7 +3816,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>80</v>
       </c>
@@ -3833,7 +3845,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>83</v>
       </c>
@@ -3862,7 +3874,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>86</v>
       </c>
@@ -3891,7 +3903,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>89</v>
       </c>
@@ -3920,7 +3932,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>92</v>
       </c>
@@ -3949,7 +3961,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>96</v>
       </c>
@@ -3978,7 +3990,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>99</v>
       </c>
@@ -4007,7 +4019,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>103</v>
       </c>
@@ -4036,7 +4048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="76" t="s">
         <v>106</v>
       </c>
@@ -4063,7 +4075,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>109</v>
       </c>
@@ -4090,7 +4102,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>112</v>
       </c>
@@ -4117,7 +4129,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>115</v>
       </c>
@@ -4144,7 +4156,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>118</v>
       </c>
@@ -4171,7 +4183,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>121</v>
       </c>
@@ -4198,7 +4210,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>124</v>
       </c>
@@ -4225,7 +4237,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>127</v>
       </c>
@@ -4252,21 +4264,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="92" t="s">
+    <row r="34" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="96" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="92"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="92"/>
-      <c r="E35" s="92"/>
-      <c r="F35" s="92"/>
-      <c r="G35" s="92"/>
-      <c r="H35" s="92"/>
-      <c r="I35" s="92"/>
-    </row>
-    <row r="36" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="96"/>
+      <c r="C35" s="96"/>
+      <c r="D35" s="96"/>
+      <c r="E35" s="96"/>
+      <c r="F35" s="96"/>
+      <c r="G35" s="96"/>
+      <c r="H35" s="96"/>
+      <c r="I35" s="96"/>
+    </row>
+    <row r="36" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>36</v>
       </c>
@@ -4295,7 +4307,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>50</v>
       </c>
@@ -4324,7 +4336,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>61</v>
       </c>
@@ -4353,7 +4365,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>77</v>
       </c>
@@ -4382,7 +4394,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>106</v>
       </c>
@@ -4409,7 +4421,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="45.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="45.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>109</v>
       </c>
@@ -4436,7 +4448,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>112</v>
       </c>
@@ -4463,7 +4475,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>115</v>
       </c>
@@ -4490,7 +4502,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>118</v>
       </c>
@@ -4517,7 +4529,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>121</v>
       </c>
@@ -4544,7 +4556,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
         <v>124</v>
       </c>
@@ -4571,7 +4583,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
         <v>127</v>
       </c>
@@ -4598,24 +4610,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J48" s="39"/>
     </row>
-    <row r="49" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="92" t="s">
+    <row r="49" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="B49" s="92"/>
-      <c r="C49" s="92"/>
-      <c r="D49" s="92"/>
-      <c r="E49" s="92"/>
-      <c r="F49" s="92"/>
-      <c r="G49" s="92"/>
-      <c r="H49" s="92"/>
-      <c r="I49" s="93"/>
+      <c r="B49" s="96"/>
+      <c r="C49" s="96"/>
+      <c r="D49" s="96"/>
+      <c r="E49" s="96"/>
+      <c r="F49" s="96"/>
+      <c r="G49" s="96"/>
+      <c r="H49" s="96"/>
+      <c r="I49" s="97"/>
       <c r="J49" s="51"/>
     </row>
-    <row r="50" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="43" t="s">
         <v>24</v>
       </c>
@@ -4644,7 +4656,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="43" t="s">
         <v>32</v>
       </c>
@@ -4673,7 +4685,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="47" t="s">
         <v>41</v>
       </c>
@@ -4702,7 +4714,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="64" t="s">
         <v>47</v>
       </c>
@@ -4731,7 +4743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="65"/>
       <c r="B54" s="55"/>
       <c r="C54" s="55"/>
@@ -4742,7 +4754,7 @@
       <c r="H54" s="59"/>
       <c r="I54" s="57"/>
     </row>
-    <row r="55" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="43" t="s">
         <v>64</v>
       </c>
@@ -4771,7 +4783,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="47" t="s">
         <v>57</v>
       </c>
@@ -4800,7 +4812,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="43" t="s">
         <v>74</v>
       </c>
@@ -4829,7 +4841,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="43" t="s">
         <v>80</v>
       </c>
@@ -4858,7 +4870,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="43" t="s">
         <v>83</v>
       </c>
@@ -4887,7 +4899,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="43" t="s">
         <v>86</v>
       </c>
@@ -4916,7 +4928,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="47" t="s">
         <v>71</v>
       </c>
@@ -4945,7 +4957,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="43" t="s">
         <v>80</v>
       </c>
@@ -4974,7 +4986,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="43" t="s">
         <v>118</v>
       </c>
@@ -5003,7 +5015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="43" t="s">
         <v>83</v>
       </c>
@@ -5032,7 +5044,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="47" t="s">
         <v>89</v>
       </c>
@@ -5061,7 +5073,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="43" t="s">
         <v>142</v>
       </c>
@@ -5090,7 +5102,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="43" t="s">
         <v>143</v>
       </c>
@@ -5119,7 +5131,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="43" t="s">
         <v>144</v>
       </c>
@@ -5148,20 +5160,20 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="94" t="s">
+    <row r="71" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="98" t="s">
         <v>145</v>
       </c>
-      <c r="B71" s="94"/>
-      <c r="C71" s="94"/>
-      <c r="D71" s="94"/>
-      <c r="E71" s="94"/>
-      <c r="F71" s="94"/>
-      <c r="G71" s="94"/>
-      <c r="H71" s="94"/>
-      <c r="I71" s="94"/>
-    </row>
-    <row r="72" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="98"/>
+      <c r="C71" s="98"/>
+      <c r="D71" s="98"/>
+      <c r="E71" s="98"/>
+      <c r="F71" s="98"/>
+      <c r="G71" s="98"/>
+      <c r="H71" s="98"/>
+      <c r="I71" s="98"/>
+    </row>
+    <row r="72" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
         <v>67</v>
       </c>
@@ -5190,7 +5202,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
         <v>80</v>
       </c>
@@ -5219,92 +5231,152 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B74" s="123" t="s">
+      <c r="B74" s="92" t="s">
         <v>236</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
-    </row>
-    <row r="75" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="D74" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F74" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G74" s="15">
+        <v>8</v>
+      </c>
+      <c r="H74" s="19">
+        <v>15</v>
+      </c>
+      <c r="I74" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B75" s="123" t="s">
+      <c r="B75" s="92" t="s">
         <v>237</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-      <c r="I75" s="9"/>
-    </row>
-    <row r="76" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="121" t="s">
+      <c r="D75" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F75" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G75" s="15">
+        <v>8</v>
+      </c>
+      <c r="H75" s="19">
+        <v>15</v>
+      </c>
+      <c r="I75" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="90" t="s">
         <v>96</v>
       </c>
-      <c r="B76" s="124" t="s">
+      <c r="B76" s="93" t="s">
         <v>238</v>
       </c>
-      <c r="C76" s="122" t="s">
-        <v>69</v>
-      </c>
-      <c r="D76" s="122"/>
-      <c r="E76" s="122"/>
-      <c r="F76" s="122"/>
-      <c r="G76" s="122"/>
-      <c r="H76" s="122"/>
-      <c r="I76" s="122"/>
-    </row>
-    <row r="77" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="91" t="s">
+        <v>246</v>
+      </c>
+      <c r="D76" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F76" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G76" s="15">
+        <v>8</v>
+      </c>
+      <c r="H76" s="19">
+        <v>15</v>
+      </c>
+      <c r="I76" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B77" s="123" t="s">
+      <c r="B77" s="92" t="s">
         <v>239</v>
       </c>
-      <c r="C77" s="122" t="s">
-        <v>69</v>
-      </c>
-      <c r="D77" s="9"/>
-      <c r="E77" s="9"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9"/>
-    </row>
-    <row r="78" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="91" t="s">
+        <v>247</v>
+      </c>
+      <c r="D77" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G77" s="15">
+        <v>8</v>
+      </c>
+      <c r="H77" s="19">
+        <v>15</v>
+      </c>
+      <c r="I77" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B78" s="123" t="s">
+      <c r="B78" s="92" t="s">
         <v>240</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9"/>
-    </row>
-    <row r="79" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="D78" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F78" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G78" s="15">
+        <v>8</v>
+      </c>
+      <c r="H78" s="19">
+        <v>15</v>
+      </c>
+      <c r="I78" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="s">
         <v>118</v>
       </c>
@@ -5314,49 +5386,78 @@
       <c r="C79" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
-      <c r="I79" s="9"/>
-    </row>
-    <row r="80" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D79" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F79" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G79" s="15">
+        <v>8</v>
+      </c>
+      <c r="H79" s="19">
+        <v>15</v>
+      </c>
+      <c r="I79" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="B80" s="123" t="s">
+      <c r="B80" s="92" t="s">
         <v>242</v>
       </c>
       <c r="C80" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
-      <c r="I80" s="9"/>
-    </row>
-    <row r="81" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D80" s="41"/>
+      <c r="E80" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F80" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G80" s="15">
+        <v>8</v>
+      </c>
+      <c r="H80" s="19">
+        <v>15</v>
+      </c>
+      <c r="I80" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B81" s="123" t="s">
+      <c r="B81" s="92" t="s">
         <v>243</v>
       </c>
       <c r="C81" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D81" s="9"/>
-      <c r="E81" s="9"/>
-      <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="9"/>
-    </row>
-    <row r="84" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C84" s="125"/>
+      <c r="D81" s="41"/>
+      <c r="E81" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F81" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G81" s="15">
+        <v>8</v>
+      </c>
+      <c r="H81" s="19">
+        <v>15</v>
+      </c>
+      <c r="I81" s="22" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -5412,60 +5513,60 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="67" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="111" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="109"/>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="109"/>
-      <c r="B3" s="110"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="111"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="112"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="113"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="113"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="115"/>
+      <c r="B4" s="116"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="116"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>147</v>
       </c>
@@ -5491,7 +5592,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>1</v>
       </c>
@@ -5517,7 +5618,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="29">
         <v>2</v>
       </c>
@@ -5543,7 +5644,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="29">
         <v>3</v>
       </c>
@@ -5569,7 +5670,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>4</v>
       </c>
@@ -5595,7 +5696,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>5</v>
       </c>
@@ -5621,7 +5722,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>6</v>
       </c>
@@ -5647,7 +5748,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>7</v>
       </c>
@@ -5673,7 +5774,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>8</v>
       </c>
@@ -5699,7 +5800,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H4"/>
@@ -5716,41 +5817,41 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" style="87" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="87" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" style="87" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="87" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" style="87" customWidth="1"/>
-    <col min="6" max="6" width="59.5703125" style="87" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" style="87" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="87"/>
+    <col min="1" max="1" width="29.44140625" style="87" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" style="87" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="87" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="87" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" style="87" customWidth="1"/>
+    <col min="6" max="6" width="59.5546875" style="87" customWidth="1"/>
+    <col min="7" max="7" width="36.5546875" style="87" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="87"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+    <row r="1" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="117" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="115"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="116" t="s">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="119"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="120" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="118"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="122"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="81" t="s">
         <v>182</v>
       </c>
@@ -5773,7 +5874,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="82" t="s">
         <v>187</v>
       </c>
@@ -5794,7 +5895,7 @@
       </c>
       <c r="G4" s="82"/>
     </row>
-    <row r="5" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>191</v>
       </c>
@@ -5815,7 +5916,7 @@
       </c>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>195</v>
       </c>
@@ -5836,7 +5937,7 @@
       </c>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="86" t="s">
         <v>198</v>
       </c>
@@ -5857,18 +5958,18 @@
       </c>
       <c r="G7" s="37"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="116" t="s">
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A8" s="120" t="s">
         <v>201</v>
       </c>
-      <c r="B8" s="119"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="120"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="123"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="124"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="81" t="s">
         <v>182</v>
       </c>
@@ -5891,7 +5992,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="82" t="s">
         <v>202</v>
       </c>
@@ -5912,7 +6013,7 @@
       </c>
       <c r="G10" s="82"/>
     </row>
-    <row r="11" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
         <v>205</v>
       </c>
@@ -5935,7 +6036,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="38" t="s">
         <v>208</v>
       </c>
@@ -5956,7 +6057,7 @@
       </c>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="86" t="s">
         <v>211</v>
       </c>
@@ -5977,18 +6078,18 @@
       </c>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="116" t="s">
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A14" s="120" t="s">
         <v>214</v>
       </c>
-      <c r="B14" s="119"/>
-      <c r="C14" s="119"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="119"/>
-      <c r="G14" s="120"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="123"/>
+      <c r="C14" s="123"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="124"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="81" t="s">
         <v>182</v>
       </c>
@@ -6011,7 +6112,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="82" t="s">
         <v>215</v>
       </c>
@@ -6032,7 +6133,7 @@
       </c>
       <c r="G16" s="82"/>
     </row>
-    <row r="17" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
         <v>216</v>
       </c>
@@ -6053,7 +6154,7 @@
       </c>
       <c r="G17" s="37"/>
     </row>
-    <row r="18" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
         <v>205</v>
       </c>
@@ -6074,7 +6175,7 @@
       </c>
       <c r="G18" s="82"/>
     </row>
-    <row r="19" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="86" t="s">
         <v>217</v>
       </c>
@@ -6095,7 +6196,7 @@
       </c>
       <c r="G19" s="37"/>
     </row>
-    <row r="20" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="38" t="s">
         <v>226</v>
       </c>
@@ -6116,7 +6217,7 @@
       </c>
       <c r="G20" s="82"/>
     </row>
-    <row r="21" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="86" t="s">
         <v>220</v>
       </c>
@@ -6137,18 +6238,18 @@
       </c>
       <c r="G21" s="37"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="116" t="s">
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A22" s="120" t="s">
         <v>229</v>
       </c>
-      <c r="B22" s="119"/>
-      <c r="C22" s="119"/>
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
-      <c r="F22" s="119"/>
-      <c r="G22" s="120"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="123"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="123"/>
+      <c r="G22" s="124"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" s="81" t="s">
         <v>182</v>
       </c>
@@ -6171,7 +6272,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="82" t="s">
         <v>230</v>
       </c>
@@ -6192,7 +6293,7 @@
       </c>
       <c r="G24" s="82"/>
     </row>
-    <row r="25" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37" t="s">
         <v>231</v>
       </c>
@@ -6213,7 +6314,7 @@
       </c>
       <c r="G25" s="37"/>
     </row>
-    <row r="26" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="38" t="s">
         <v>232</v>
       </c>
@@ -6234,7 +6335,7 @@
       </c>
       <c r="G26" s="82"/>
     </row>
-    <row r="27" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="86" t="s">
         <v>233</v>
       </c>
@@ -6255,7 +6356,7 @@
       </c>
       <c r="G27" s="37"/>
     </row>
-    <row r="28" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="88" t="s">
         <v>234</v>
       </c>

</xml_diff>